<commit_message>
More work on demographic counts
</commit_message>
<xml_diff>
--- a/raw/Survey Key.xlsx
+++ b/raw/Survey Key.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gclawson/Desktop/PangaWatch/survey_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A975FF6C-0F5E-F344-A051-A7EEC3F1D0BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="28140" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18075" yWindow="0" windowWidth="9585" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Column Key" sheetId="1" r:id="rId1"/>
     <sheet name="Choices" sheetId="3" r:id="rId2"/>
     <sheet name="Full Question" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="561">
   <si>
     <t>Question</t>
   </si>
@@ -1563,9 +1557,6 @@
     <t>Severe</t>
   </si>
   <si>
-    <t>34.i.ii.iii.iv.</t>
-  </si>
-  <si>
     <t>iuu</t>
   </si>
   <si>
@@ -1706,11 +1697,14 @@
   <si>
     <t>MAK</t>
   </si>
+  <si>
+    <t>34..iii.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -2027,18 +2021,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C16385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -68326,20 +68320,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -68682,7 +68676,7 @@
     <row r="32" spans="1:4" ht="15.75" customHeight="1">
       <c r="A32" s="1"/>
       <c r="C32" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>308</v>
@@ -69697,7 +69691,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="13">
+    <row r="126" spans="1:4" ht="12.75">
       <c r="C126" s="5" t="s">
         <v>496</v>
       </c>
@@ -69705,7 +69699,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="13">
+    <row r="127" spans="1:4" ht="12.75">
       <c r="C127" s="5" t="s">
         <v>498</v>
       </c>
@@ -69713,7 +69707,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="13">
+    <row r="128" spans="1:4" ht="12.75">
       <c r="C128" s="5" t="s">
         <v>500</v>
       </c>
@@ -69721,7 +69715,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="13">
+    <row r="129" spans="1:4" ht="12.75">
       <c r="C129" s="5" t="s">
         <v>502</v>
       </c>
@@ -69729,7 +69723,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="13">
+    <row r="130" spans="1:4" ht="12.75">
       <c r="C130" s="5" t="s">
         <v>480</v>
       </c>
@@ -69872,43 +69866,49 @@
     </row>
     <row r="145" spans="1:4" ht="15">
       <c r="A145" s="19" t="s">
-        <v>513</v>
+        <v>189</v>
       </c>
       <c r="B145" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C145" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="D145" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="D145" s="5" t="s">
+    </row>
+    <row r="146" spans="1:4" ht="15">
+      <c r="A146" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C146" s="5" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" ht="15">
-      <c r="A146" s="13"/>
-      <c r="C146" s="5" t="s">
+      <c r="D146" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D146" s="5" t="s">
+    </row>
+    <row r="147" spans="1:4" ht="15">
+      <c r="A147" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="C147" s="5" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="15">
-      <c r="A147" s="13"/>
-      <c r="C147" s="5" t="s">
+      <c r="D147" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="D147" s="5" t="s">
+    </row>
+    <row r="148" spans="1:4" ht="15">
+      <c r="A148" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C148" s="5" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" ht="15">
-      <c r="A148" s="13"/>
-      <c r="C148" s="5" t="s">
+      <c r="D148" s="5" t="s">
         <v>520</v>
-      </c>
-      <c r="D148" s="5" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15">
@@ -69919,51 +69919,51 @@
         <v>107</v>
       </c>
       <c r="C149" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="D149" s="5" t="s">
         <v>522</v>
-      </c>
-      <c r="D149" s="5" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15">
       <c r="A150" s="13"/>
       <c r="C150" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="D150" s="5" t="s">
         <v>524</v>
-      </c>
-      <c r="D150" s="5" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15">
       <c r="A151" s="13"/>
       <c r="C151" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="D151" s="5" t="s">
         <v>526</v>
-      </c>
-      <c r="D151" s="5" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15">
       <c r="A152" s="13"/>
       <c r="C152" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="D152" s="5" t="s">
         <v>528</v>
-      </c>
-      <c r="D152" s="5" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15">
       <c r="A153" s="13"/>
       <c r="C153" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="D153" s="5" t="s">
         <v>530</v>
-      </c>
-      <c r="D153" s="5" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15">
       <c r="A154" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>107</v>
@@ -69972,7 +69972,7 @@
         <v>1</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15">
@@ -69981,7 +69981,7 @@
         <v>2</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15">
@@ -69990,7 +69990,7 @@
         <v>3</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15">
@@ -69999,7 +69999,7 @@
         <v>4</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15">
@@ -70008,12 +70008,12 @@
         <v>5</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15">
       <c r="A159" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>107</v>
@@ -70022,7 +70022,7 @@
         <v>1</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15">
@@ -70031,7 +70031,7 @@
         <v>2</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15">
@@ -70040,7 +70040,7 @@
         <v>3</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15">
@@ -70049,7 +70049,7 @@
         <v>4</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15">
@@ -70058,12 +70058,12 @@
         <v>5</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15">
       <c r="A164" s="19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>107</v>
@@ -70072,7 +70072,7 @@
         <v>1</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15">
@@ -70081,7 +70081,7 @@
         <v>2</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15">
@@ -70090,7 +70090,7 @@
         <v>3</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15">
@@ -70099,7 +70099,7 @@
         <v>4</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15">
@@ -70108,7 +70108,7 @@
         <v>5</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15">
@@ -70118,7 +70118,7 @@
         <v>0</v>
       </c>
       <c r="D169" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15">
@@ -70145,45 +70145,45 @@
         <v>107</v>
       </c>
       <c r="C172" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="D172" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="D172" s="4" t="s">
+    </row>
+    <row r="173" spans="1:4" ht="12.75">
+      <c r="C173" s="5" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" ht="13">
-      <c r="C173" s="5" t="s">
+      <c r="D173" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="D173" s="4" t="s">
+    </row>
+    <row r="174" spans="1:4" ht="12.75">
+      <c r="C174" s="5" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" ht="13">
-      <c r="C174" s="5" t="s">
+      <c r="D174" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="D174" s="4" t="s">
+    </row>
+    <row r="175" spans="1:4" ht="12.75">
+      <c r="C175" s="5" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" ht="13">
-      <c r="C175" s="5" t="s">
+      <c r="D175" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="D175" s="4" t="s">
+    </row>
+    <row r="176" spans="1:4" ht="12.75">
+      <c r="C176" s="5" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" ht="13">
-      <c r="C176" s="5" t="s">
+      <c r="D176" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="D176" s="4" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="13">
+    </row>
+    <row r="177" spans="1:4" ht="12.75">
       <c r="C177" s="5" t="s">
         <v>480</v>
       </c>
@@ -70243,7 +70243,7 @@
         <v>391</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15">
@@ -70260,18 +70260,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">

</xml_diff>